<commit_message>
Updated VLMD hardcoded version
</commit_message>
<xml_diff>
--- a/CDE_ID_detective_revamp/Data_Dictionary_Tracker_as_of_2025-07-08.xlsx
+++ b/CDE_ID_detective_revamp/Data_Dictionary_Tracker_as_of_2025-07-08.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmaefos\Code Stuffs\CDE_detective\CDE_ID_detective_revamp\ReRun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmbfo\CDE_detective\CDE_ID_detective_revamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC507673-1E1D-46A7-B187-B773A58CD56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3AA818-B3FF-4340-8AD0-F2D64C051283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="7110" windowWidth="15915" windowHeight="18480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data dictionary track" sheetId="1" r:id="rId1"/>
@@ -2175,7 +2175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2393,26 +2393,19 @@
     <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2433,50 +2426,23 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2809,58 +2775,55 @@
   <dimension ref="A1:AN58"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="23" ySplit="2" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA52" sqref="AA52"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.8125" customWidth="1"/>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="36.3125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.3125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="42.875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="36.3125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="96.8125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="33" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="28.0625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="9.875" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.609375" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="42.88671875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="96.83203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="33" customWidth="1"/>
+    <col min="14" max="14" width="28.0546875" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="16.5" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="18.125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="19.8125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="18.6875" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="24.1875" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="25.3125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="17.625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="18.109375" customWidth="1"/>
+    <col min="19" max="19" width="19.83203125" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="24.1640625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="25.33203125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="17.609375" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="20" customWidth="1"/>
-    <col min="25" max="25" width="19.8125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="72.75" customWidth="1"/>
-    <col min="27" max="27" width="100.4375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="78.4375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.1875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5625" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="36.3125" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5625" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="13.1875" hidden="1" customWidth="1"/>
-    <col min="35" max="39" width="36.3125" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="37.375" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="72.71875" customWidth="1"/>
+    <col min="27" max="27" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="78.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31.38671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5546875" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5546875" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="13.1640625" hidden="1" customWidth="1"/>
+    <col min="35" max="39" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="37.38671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:40" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="28" t="s">
         <v>341</v>
       </c>
@@ -2912,7 +2875,7 @@
       <c r="Q2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="88" t="s">
         <v>18</v>
       </c>
       <c r="S2" s="3" t="s">
@@ -2982,7 +2945,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
@@ -3056,13 +3019,13 @@
       <c r="Y3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Z3" s="76" t="s">
+      <c r="Z3" s="75" t="s">
         <v>343</v>
       </c>
-      <c r="AA3" s="87" t="s">
+      <c r="AA3" s="84" t="s">
         <v>412</v>
       </c>
-      <c r="AB3" s="77"/>
+      <c r="AB3" s="6"/>
       <c r="AC3" s="12" t="s">
         <v>53</v>
       </c>
@@ -3100,7 +3063,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="29" t="s">
         <v>2</v>
       </c>
@@ -3176,9 +3139,9 @@
       <c r="Y4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="73"/>
       <c r="AC4" s="49"/>
       <c r="AD4" s="13" t="s">
         <v>54</v>
@@ -3214,7 +3177,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="29" t="s">
         <v>2</v>
       </c>
@@ -3291,7 +3254,7 @@
       <c r="Z5" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="AA5" s="85" t="s">
+      <c r="AA5" s="82" t="s">
         <v>414</v>
       </c>
       <c r="AB5" s="31"/>
@@ -3332,7 +3295,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
@@ -3411,7 +3374,7 @@
       <c r="Z6" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="AA6" s="86" t="s">
+      <c r="AA6" s="83" t="s">
         <v>436</v>
       </c>
       <c r="AB6" s="6"/>
@@ -3452,7 +3415,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="29" t="s">
         <v>2</v>
       </c>
@@ -3528,13 +3491,13 @@
       <c r="Y7" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="Z7" s="77" t="s">
+      <c r="Z7" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="AA7" s="80" t="s">
+      <c r="AA7" s="69" t="s">
         <v>415</v>
       </c>
-      <c r="AB7" s="77"/>
+      <c r="AB7" s="6"/>
       <c r="AC7" s="12" t="s">
         <v>53</v>
       </c>
@@ -3566,7 +3529,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="29" t="s">
         <v>2</v>
       </c>
@@ -3674,7 +3637,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="29" t="s">
         <v>2</v>
       </c>
@@ -3751,7 +3714,7 @@
       <c r="Z9" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="AA9" s="86" t="s">
+      <c r="AA9" s="83" t="s">
         <v>418</v>
       </c>
       <c r="AB9" s="6"/>
@@ -3786,7 +3749,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="29" t="s">
         <v>2</v>
       </c>
@@ -3862,12 +3825,12 @@
       <c r="Y10" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="Z10" s="75" t="s">
+      <c r="Z10" s="74" t="s">
         <v>360</v>
       </c>
-      <c r="AA10" s="75"/>
-      <c r="AB10" s="75"/>
-      <c r="AC10" s="81" t="s">
+      <c r="AA10" s="74"/>
+      <c r="AB10" s="74"/>
+      <c r="AC10" s="78" t="s">
         <v>117</v>
       </c>
       <c r="AD10" s="13" t="s">
@@ -3904,7 +3867,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="29" t="s">
         <v>2</v>
       </c>
@@ -3983,7 +3946,7 @@
       <c r="Z11" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="AA11" s="86" t="s">
+      <c r="AA11" s="83" t="s">
         <v>425</v>
       </c>
       <c r="AB11" s="6"/>
@@ -4018,7 +3981,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="29" t="s">
         <v>2</v>
       </c>
@@ -4088,8 +4051,8 @@
         <v>1</v>
       </c>
       <c r="Y12" s="24"/>
-      <c r="Z12" s="84"/>
-      <c r="AA12" s="74"/>
+      <c r="Z12" s="81"/>
+      <c r="AA12" s="73"/>
       <c r="AB12" s="63"/>
       <c r="AC12" s="17"/>
       <c r="AD12" s="13" t="s">
@@ -4122,7 +4085,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="29" t="s">
         <v>2</v>
       </c>
@@ -4201,7 +4164,7 @@
       <c r="Z13" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="AA13" s="86" t="s">
+      <c r="AA13" s="83" t="s">
         <v>422</v>
       </c>
       <c r="AB13" s="6"/>
@@ -4238,7 +4201,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="29" t="s">
         <v>2</v>
       </c>
@@ -4317,7 +4280,7 @@
       <c r="Z14" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="AA14" s="88" t="s">
+      <c r="AA14" s="85" t="s">
         <v>427</v>
       </c>
       <c r="AB14" s="6"/>
@@ -4352,7 +4315,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="29" t="s">
         <v>2</v>
       </c>
@@ -4431,7 +4394,7 @@
       <c r="Z15" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="AA15" s="86" t="s">
+      <c r="AA15" s="83" t="s">
         <v>429</v>
       </c>
       <c r="AB15" s="6"/>
@@ -4466,7 +4429,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="29" t="s">
         <v>2</v>
       </c>
@@ -4543,7 +4506,7 @@
       <c r="Z16" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="AA16" s="86" t="s">
+      <c r="AA16" s="83" t="s">
         <v>430</v>
       </c>
       <c r="AB16" s="6"/>
@@ -4584,7 +4547,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="29" t="s">
         <v>2</v>
       </c>
@@ -4660,13 +4623,13 @@
       <c r="Y17" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="Z17" s="77" t="s">
+      <c r="Z17" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="AA17" s="89" t="s">
+      <c r="AA17" s="83" t="s">
         <v>431</v>
       </c>
-      <c r="AB17" s="77"/>
+      <c r="AB17" s="6"/>
       <c r="AC17" s="12" t="s">
         <v>53</v>
       </c>
@@ -4704,7 +4667,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="29" t="s">
         <v>2</v>
       </c>
@@ -4726,7 +4689,7 @@
       <c r="G18" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="82" t="s">
+      <c r="H18" s="79" t="s">
         <v>42</v>
       </c>
       <c r="I18" s="5">
@@ -4778,13 +4741,13 @@
       <c r="Y18" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="Z18" s="77" t="s">
+      <c r="Z18" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="AA18" s="89" t="s">
+      <c r="AA18" s="83" t="s">
         <v>424</v>
       </c>
-      <c r="AB18" s="77"/>
+      <c r="AB18" s="6"/>
       <c r="AC18" s="12" t="s">
         <v>53</v>
       </c>
@@ -4816,7 +4779,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="29" t="s">
         <v>2</v>
       </c>
@@ -4892,13 +4855,13 @@
       <c r="Y19" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Z19" s="77" t="s">
+      <c r="Z19" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="AA19" s="89" t="s">
+      <c r="AA19" s="83" t="s">
         <v>426</v>
       </c>
-      <c r="AB19" s="77"/>
+      <c r="AB19" s="6"/>
       <c r="AC19" s="12" t="s">
         <v>53</v>
       </c>
@@ -4936,7 +4899,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -5008,13 +4971,13 @@
       <c r="Y20" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="Z20" s="76" t="s">
+      <c r="Z20" s="75" t="s">
         <v>362</v>
       </c>
-      <c r="AA20" s="87" t="s">
+      <c r="AA20" s="84" t="s">
         <v>409</v>
       </c>
-      <c r="AB20" s="77"/>
+      <c r="AB20" s="6"/>
       <c r="AC20" s="12" t="s">
         <v>53</v>
       </c>
@@ -5052,7 +5015,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -5127,7 +5090,7 @@
       <c r="Z21" s="47" t="s">
         <v>361</v>
       </c>
-      <c r="AA21" s="85" t="s">
+      <c r="AA21" s="82" t="s">
         <v>410</v>
       </c>
       <c r="AB21" s="31"/>
@@ -5168,7 +5131,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -5270,7 +5233,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -5372,7 +5335,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -5438,9 +5401,9 @@
         <v>1</v>
       </c>
       <c r="Y24" s="62"/>
-      <c r="Z24" s="77"/>
+      <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
-      <c r="AB24" s="77"/>
+      <c r="AB24" s="6"/>
       <c r="AC24" s="49"/>
       <c r="AD24" s="13" t="s">
         <v>54</v>
@@ -5474,7 +5437,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -5574,7 +5537,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="26" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -5676,7 +5639,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -5778,7 +5741,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -5882,7 +5845,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="29" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -5956,12 +5919,12 @@
       <c r="Y29" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="Z29" s="75" t="s">
+      <c r="Z29" s="74" t="s">
         <v>360</v>
       </c>
-      <c r="AA29" s="75"/>
-      <c r="AB29" s="75"/>
-      <c r="AC29" s="81" t="s">
+      <c r="AA29" s="74"/>
+      <c r="AB29" s="74"/>
+      <c r="AC29" s="78" t="s">
         <v>117</v>
       </c>
       <c r="AD29" s="13" t="s">
@@ -5998,7 +5961,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -6100,7 +6063,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="31" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -6172,13 +6135,13 @@
       <c r="Y31" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="Z31" s="77" t="s">
+      <c r="Z31" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="AA31" s="89" t="s">
+      <c r="AA31" s="83" t="s">
         <v>416</v>
       </c>
-      <c r="AB31" s="77"/>
+      <c r="AB31" s="6"/>
       <c r="AC31" s="12" t="s">
         <v>53</v>
       </c>
@@ -6216,7 +6179,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -6320,7 +6283,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="33" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -6422,7 +6385,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -6501,7 +6464,7 @@
       <c r="Z34" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="AA34" s="86" t="s">
+      <c r="AA34" s="83" t="s">
         <v>417</v>
       </c>
       <c r="AB34" s="6"/>
@@ -6536,7 +6499,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -6640,7 +6603,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -6711,13 +6674,13 @@
       <c r="X36" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="Y36" s="83" t="s">
+      <c r="Y36" s="80" t="s">
         <v>52</v>
       </c>
       <c r="Z36" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="AA36" s="86" t="s">
+      <c r="AA36" s="83" t="s">
         <v>419</v>
       </c>
       <c r="AB36" s="6"/>
@@ -6758,7 +6721,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -6829,16 +6792,16 @@
       <c r="X37" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="Y37" s="83" t="s">
+      <c r="Y37" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="Z37" s="77" t="s">
+      <c r="Z37" s="6" t="s">
         <v>358</v>
       </c>
       <c r="AA37" s="69" t="s">
         <v>420</v>
       </c>
-      <c r="AB37" s="77"/>
+      <c r="AB37" s="6"/>
       <c r="AC37" s="12" t="s">
         <v>53</v>
       </c>
@@ -6876,7 +6839,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -6953,7 +6916,7 @@
       <c r="Z38" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="AA38" s="86" t="s">
+      <c r="AA38" s="83" t="s">
         <v>421</v>
       </c>
       <c r="AB38" s="6"/>
@@ -6988,7 +6951,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="39" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -7059,16 +7022,16 @@
       <c r="X39" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="Y39" s="83" t="s">
+      <c r="Y39" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="Z39" s="79" t="s">
+      <c r="Z39" s="77" t="s">
         <v>364</v>
       </c>
-      <c r="AA39" s="90" t="s">
+      <c r="AA39" s="86" t="s">
         <v>413</v>
       </c>
-      <c r="AB39" s="77"/>
+      <c r="AB39" s="6"/>
       <c r="AC39" s="12" t="s">
         <v>53</v>
       </c>
@@ -7106,7 +7069,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="40" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -7210,7 +7173,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="41" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -7287,7 +7250,7 @@
       <c r="Z41" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="AA41" s="86" t="s">
+      <c r="AA41" s="83" t="s">
         <v>423</v>
       </c>
       <c r="AB41" s="6"/>
@@ -7324,7 +7287,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -7424,7 +7387,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="43" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -7501,7 +7464,7 @@
       <c r="Z43" s="31" t="s">
         <v>405</v>
       </c>
-      <c r="AA43" s="85" t="s">
+      <c r="AA43" s="82" t="s">
         <v>428</v>
       </c>
       <c r="AB43" s="31"/>
@@ -7536,7 +7499,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="44" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -7640,7 +7603,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="45" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -7717,7 +7680,7 @@
       <c r="Z45" s="31" t="s">
         <v>403</v>
       </c>
-      <c r="AA45" s="85" t="s">
+      <c r="AA45" s="82" t="s">
         <v>432</v>
       </c>
       <c r="AB45" s="31"/>
@@ -7752,7 +7715,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="46" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -7826,10 +7789,10 @@
       <c r="Y46" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="Z46" s="78" t="s">
+      <c r="Z46" s="76" t="s">
         <v>404</v>
       </c>
-      <c r="AA46" s="85" t="s">
+      <c r="AA46" s="82" t="s">
         <v>433</v>
       </c>
       <c r="AB46" s="31"/>
@@ -7864,7 +7827,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -7968,7 +7931,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="48" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -8045,7 +8008,7 @@
       <c r="Z48" s="31" t="s">
         <v>363</v>
       </c>
-      <c r="AA48" s="85" t="s">
+      <c r="AA48" s="82" t="s">
         <v>434</v>
       </c>
       <c r="AB48" s="31"/>
@@ -8086,7 +8049,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -8202,7 +8165,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -8316,7 +8279,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="51" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -8432,7 +8395,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="52" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -8546,7 +8509,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -8660,7 +8623,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="54" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -8774,7 +8737,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -8890,7 +8853,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="56" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -8967,7 +8930,7 @@
       <c r="Z56" s="68" t="s">
         <v>401</v>
       </c>
-      <c r="AA56" s="91" t="s">
+      <c r="AA56" s="87" t="s">
         <v>411</v>
       </c>
       <c r="AB56" s="31"/>
@@ -9008,7 +8971,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:40" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -9085,7 +9048,7 @@
       <c r="Z57" s="31" t="s">
         <v>399</v>
       </c>
-      <c r="AA57" s="85" t="s">
+      <c r="AA57" s="82" t="s">
         <v>435</v>
       </c>
       <c r="AB57" s="31"/>
@@ -9126,7 +9089,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="58" spans="1:40" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:40" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
         <v>1</v>
       </c>
@@ -9145,7 +9108,7 @@
       <c r="G58" t="s">
         <v>1</v>
       </c>
-      <c r="H58" s="73" t="s">
+      <c r="H58" t="s">
         <v>1</v>
       </c>
       <c r="I58" s="26" t="s">
@@ -9166,13 +9129,13 @@
       <c r="N58" t="s">
         <v>1</v>
       </c>
-      <c r="O58" s="73" t="s">
+      <c r="O58" t="s">
         <v>1</v>
       </c>
       <c r="P58" t="s">
         <v>1</v>
       </c>
-      <c r="Q58" s="73" t="s">
+      <c r="Q58" t="s">
         <v>1</v>
       </c>
       <c r="R58" t="s">
@@ -9190,34 +9153,31 @@
       <c r="V58" t="s">
         <v>1</v>
       </c>
-      <c r="W58" s="73" t="s">
+      <c r="W58" t="s">
         <v>1</v>
       </c>
       <c r="X58" t="s">
         <v>1</v>
       </c>
-      <c r="Y58" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z58" s="73"/>
-      <c r="AA58" s="73"/>
-      <c r="AB58" s="73"/>
-      <c r="AC58" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD58" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE58" s="73" t="s">
+      <c r="Y58" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD58" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE58" t="s">
         <v>1</v>
       </c>
       <c r="AF58" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="AG58" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH58" s="73" t="s">
+      <c r="AG58" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH58" t="s">
         <v>1</v>
       </c>
       <c r="AI58" s="26" t="s">

</xml_diff>